<commit_message>
Created Dyno Harness (not including Data Logger)
</commit_message>
<xml_diff>
--- a/harness/excelSheets/q20_dynoHarness.xlsx
+++ b/harness/excelSheets/q20_dynoHarness.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Desktop\formula\Q20\harness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick Kroeger\Documents\Formula Team\Q20\harness\excelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8505D909-1406-496D-9B8D-B050AED3A5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03CC650-3162-4CBA-8CEB-DCA4719E115B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1638" yWindow="1536" windowWidth="6120" windowHeight="3048" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4296" yWindow="420" windowWidth="17280" windowHeight="8916" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDM" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="435">
   <si>
     <t>A11</t>
   </si>
@@ -1271,9 +1271,6 @@
     <t>To GND Node</t>
   </si>
   <si>
-    <t>To ETB</t>
-  </si>
-  <si>
     <t>To Control Box</t>
   </si>
   <si>
@@ -1371,6 +1368,21 @@
   </si>
   <si>
     <t>From ETC/Shifting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>M-27</t>
+  </si>
+  <si>
+    <t>DigIn6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kill fuel/ignition </t>
+  </si>
+  <si>
+    <t>Comm2</t>
   </si>
 </sst>
 </file>
@@ -1606,9 +1618,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1618,75 +1627,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="96">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3649,6 +3597,65 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -3818,6 +3825,11 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3838,19 +3850,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G24" totalsRowShown="0" headerRowDxfId="0" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G24" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:G24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
     <sortCondition ref="A1:A24"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Pin" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Signal" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Function" dataDxfId="92"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="To/From" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Pin" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Signal" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Function" dataDxfId="91"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="To/From" dataDxfId="90"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="NOTES"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fuse" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{6DFCA7D8-4250-4344-80E1-1602B4F3D81B}" name="Voltage" dataDxfId="89"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fuse" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{6DFCA7D8-4250-4344-80E1-1602B4F3D81B}" name="Voltage" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3902,38 +3914,38 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table11" displayName="Table11" ref="A1:G9" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table11" displayName="Table11" ref="A1:G9" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A1:G9" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Pin" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Signal" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Function" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="To/From" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Location" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="RH" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="Notes" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Pin" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Signal" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Function" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="To/From" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Location" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="RH" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="Notes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table9" displayName="Table9" ref="A2:J23" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table9" displayName="Table9" ref="A2:J23" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A2:J23" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Pin" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Signal" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Function" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="To/From" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Location" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="RH" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="Notes" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="Wired In" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="Connector A Female" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="Connector B" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Pin" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Signal" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Function" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="To/From" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Location" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="RH" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="Wired In" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="Connector A Female" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="Connector B" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4013,7 +4025,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table10" displayName="Table10" ref="A1:F16" totalsRowShown="0" headerRowDxfId="88" headerRowBorderDxfId="87" tableBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table10" displayName="Table10" ref="A1:F16" totalsRowShown="0" headerRowDxfId="87" headerRowBorderDxfId="86" tableBorderDxfId="85">
   <autoFilter ref="A1:F16" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F16">
     <sortCondition ref="A1:A16"/>
@@ -4023,7 +4035,7 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Signal"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Function"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Car Use"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="To/From" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="To/From" dataDxfId="84"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4045,17 +4057,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:E31" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
-  <autoFilter ref="A1:E31" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:E32" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:E32" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
     <sortCondition ref="B1:B31"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pin" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Signal" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Function" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="To/From" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pin" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Signal" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Function" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="To/From" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Notes" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4076,70 +4088,70 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table21" displayName="Table21" ref="A12:E19" totalsRowShown="0" headerRowDxfId="84" dataDxfId="82" headerRowBorderDxfId="83" tableBorderDxfId="81" totalsRowBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table21" displayName="Table21" ref="A12:E19" totalsRowShown="0" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75" tableBorderDxfId="73" totalsRowBorderDxfId="72">
   <autoFilter ref="A12:E19" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Pin" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Signal" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Function" dataDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="To/From" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Location" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Pin" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Signal" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Function" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="To/From" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Location" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table13" displayName="Table13" ref="A2:E9" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71" totalsRowBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table13" displayName="Table13" ref="A2:E9" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
   <autoFilter ref="A2:E9" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Pin" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Signal" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Function" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="To/From" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Location" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Pin" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Signal" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Function" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="To/From" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Location" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table1320" displayName="Table1320" ref="A26:E34" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table1320" displayName="Table1320" ref="A26:E34" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A26:E34" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Pin" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Signal" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Function" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="To/From" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Location" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Pin" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Signal" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Function" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="To/From" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Location" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table132025" displayName="Table132025" ref="G26:K32" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table132025" displayName="Table132025" ref="G26:K32" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="G26:K32" xr:uid="{00000000-0009-0000-0100-000018000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Pin" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Signal" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Function" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="To/From" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Location" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Pin" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Signal" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Function" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="To/From" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Location" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table13202527" displayName="Table13202527" ref="M26:Q32" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table13202527" displayName="Table13202527" ref="M26:Q32" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="M26:Q32" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Pin" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Signal" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Function" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="To/From" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Location" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Pin" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Signal" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Function" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="To/From" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Location" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4424,32 +4436,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.68359375" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="14.05078125" style="30" customWidth="1"/>
-    <col min="8" max="8" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="30" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>28</v>
       </c>
@@ -4465,17 +4477,17 @@
       <c r="E1" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="37" t="s">
         <v>389</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="37" t="s">
         <v>390</v>
       </c>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -4486,10 +4498,10 @@
         <v>388</v>
       </c>
       <c r="D2" t="s">
-        <v>397</v>
+        <v>430</v>
       </c>
       <c r="E2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>13</v>
@@ -4499,7 +4511,7 @@
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4510,7 +4522,7 @@
         <v>391</v>
       </c>
       <c r="D3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E3" t="s">
         <v>330</v>
@@ -4523,7 +4535,7 @@
       <c r="J3"/>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -4543,7 +4555,7 @@
       <c r="J4"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -4554,7 +4566,7 @@
         <v>281</v>
       </c>
       <c r="D5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E5" t="s">
         <v>363</v>
@@ -4567,7 +4579,7 @@
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -4578,7 +4590,7 @@
         <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>13</v>
@@ -4588,7 +4600,7 @@
       <c r="J6"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -4602,7 +4614,7 @@
         <v>348</v>
       </c>
       <c r="E7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>14</v>
@@ -4612,7 +4624,7 @@
       <c r="J7"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -4623,7 +4635,7 @@
         <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>13</v>
@@ -4633,7 +4645,7 @@
       <c r="J8"/>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4641,13 +4653,13 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
+        <v>404</v>
+      </c>
+      <c r="D9" t="s">
         <v>405</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>406</v>
-      </c>
-      <c r="E9" t="s">
-        <v>407</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>14</v>
@@ -4657,7 +4669,7 @@
       <c r="J9"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -4668,7 +4680,7 @@
         <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>14</v>
@@ -4678,7 +4690,7 @@
       <c r="J10"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -4699,7 +4711,7 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -4718,7 +4730,7 @@
       <c r="J12"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -4737,7 +4749,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -4758,7 +4770,7 @@
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -4777,7 +4789,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -4793,7 +4805,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -4812,7 +4824,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -4823,7 +4835,7 @@
         <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>13</v>
@@ -4833,7 +4845,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -4844,10 +4856,10 @@
         <v>306</v>
       </c>
       <c r="D19" t="s">
+        <v>412</v>
+      </c>
+      <c r="E19" t="s">
         <v>413</v>
-      </c>
-      <c r="E19" t="s">
-        <v>414</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>13</v>
@@ -4857,7 +4869,7 @@
       <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -4878,7 +4890,7 @@
       <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -4895,7 +4907,7 @@
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -4903,10 +4915,10 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="31"/>
@@ -4914,7 +4926,7 @@
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -4922,10 +4934,10 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D23" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="31"/>
@@ -4933,7 +4945,7 @@
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>230</v>
       </c>
@@ -4941,13 +4953,13 @@
         <v>309</v>
       </c>
       <c r="C24" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D24" t="s">
+        <v>407</v>
+      </c>
+      <c r="E24" t="s">
         <v>408</v>
-      </c>
-      <c r="E24" t="s">
-        <v>409</v>
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="31"/>
@@ -4955,192 +4967,192 @@
       <c r="J24"/>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I39"/>
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I40"/>
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I41"/>
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I42"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I45"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I46"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I47"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I48"/>
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I49"/>
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I50"/>
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I51"/>
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I56"/>
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I57"/>
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I58"/>
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I59"/>
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I60"/>
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I61"/>
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I62"/>
       <c r="J62"/>
       <c r="K62"/>
@@ -5162,23 +5174,23 @@
       <selection activeCell="I12" sqref="I12:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="29.62890625" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.41796875" customWidth="1"/>
-    <col min="9" max="10" width="10.83984375" customWidth="1"/>
-    <col min="11" max="11" width="22.26171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -5199,7 +5211,7 @@
       </c>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7</v>
       </c>
@@ -5216,7 +5228,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -5233,7 +5245,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>9</v>
       </c>
@@ -5250,7 +5262,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>17</v>
       </c>
@@ -5270,7 +5282,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>18</v>
       </c>
@@ -5290,7 +5302,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>23</v>
       </c>
@@ -5307,7 +5319,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>24</v>
       </c>
@@ -5324,7 +5336,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>27</v>
       </c>
@@ -5338,7 +5350,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>28</v>
       </c>
@@ -5352,7 +5364,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>67</v>
       </c>
@@ -5368,7 +5380,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>68</v>
       </c>
@@ -5381,7 +5393,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>73</v>
       </c>
@@ -5395,10 +5407,10 @@
         <v>314</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>74</v>
       </c>
@@ -5412,10 +5424,10 @@
         <v>314</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>77</v>
       </c>
@@ -5427,10 +5439,10 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>78</v>
       </c>
@@ -5443,23 +5455,23 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>129</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>248</v>
       </c>
@@ -5475,26 +5487,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7890625" customWidth="1"/>
-    <col min="2" max="2" width="23.41796875" customWidth="1"/>
-    <col min="3" max="3" width="23.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.89453125" customWidth="1"/>
-    <col min="5" max="5" width="26.26171875" customWidth="1"/>
-    <col min="6" max="6" width="24.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -5511,7 +5523,7 @@
       </c>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>43</v>
       </c>
@@ -5522,26 +5534,26 @@
         <v>215</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E2" s="26"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>423</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>424</v>
-      </c>
       <c r="D3" s="26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E3" s="26"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>33</v>
       </c>
@@ -5549,14 +5561,14 @@
         <v>177</v>
       </c>
       <c r="C4" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>426</v>
-      </c>
       <c r="E4" s="26"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>38</v>
       </c>
@@ -5569,7 +5581,7 @@
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>101</v>
       </c>
@@ -5582,7 +5594,7 @@
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>102</v>
       </c>
@@ -5595,7 +5607,7 @@
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>46</v>
       </c>
@@ -5609,7 +5621,7 @@
       <c r="E8" s="26"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>47</v>
       </c>
@@ -5622,7 +5634,7 @@
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>96</v>
       </c>
@@ -5637,7 +5649,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>36</v>
       </c>
@@ -5650,7 +5662,7 @@
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>32</v>
       </c>
@@ -5663,7 +5675,7 @@
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>42</v>
       </c>
@@ -5676,7 +5688,7 @@
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>104</v>
       </c>
@@ -5689,7 +5701,7 @@
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>103</v>
       </c>
@@ -5702,7 +5714,7 @@
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>93</v>
       </c>
@@ -5715,7 +5727,7 @@
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>39</v>
       </c>
@@ -5728,7 +5740,7 @@
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>41</v>
       </c>
@@ -5741,7 +5753,7 @@
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>100</v>
       </c>
@@ -5752,12 +5764,12 @@
         <v>86</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E19" s="26"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>30</v>
       </c>
@@ -5771,7 +5783,7 @@
       <c r="E20" s="26"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>95</v>
       </c>
@@ -5786,7 +5798,7 @@
       </c>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>44</v>
       </c>
@@ -5797,11 +5809,11 @@
         <v>68</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E22" s="26"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>45</v>
       </c>
@@ -5812,11 +5824,11 @@
         <v>69</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
         <v>98</v>
       </c>
@@ -5827,11 +5839,11 @@
         <v>63</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E24" s="26"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>99</v>
       </c>
@@ -5842,11 +5854,11 @@
         <v>64</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
         <v>97</v>
       </c>
@@ -5859,7 +5871,7 @@
       <c r="D26" s="26"/>
       <c r="E26" s="26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
         <v>34</v>
       </c>
@@ -5872,7 +5884,7 @@
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
         <v>35</v>
       </c>
@@ -5885,7 +5897,7 @@
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>94</v>
       </c>
@@ -5898,7 +5910,7 @@
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>31</v>
       </c>
@@ -5909,11 +5921,11 @@
         <v>54</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E30" s="26"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
         <v>40</v>
       </c>
@@ -5924,9 +5936,24 @@
         <v>60</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>434</v>
+      </c>
+      <c r="E32" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5945,222 +5972,222 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.26171875" customWidth="1"/>
-    <col min="2" max="2" width="17.9453125" customWidth="1"/>
-    <col min="3" max="3" width="14.1015625" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>352</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="34">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="35">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="34">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="35">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="34">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="35">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="34">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="35">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="34">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="35">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="34">
         <v>6</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="35">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="34">
         <v>7</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="35">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="34">
         <v>8</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="34" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="32" t="s">
         <v>352</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="32" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="34">
         <v>1</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="35">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="34">
         <v>2</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="35">
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="34">
         <v>3</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="35">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="34">
         <v>4</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="35">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="34">
         <v>5</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="35">
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="34">
         <v>6</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="35">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="34">
         <v>7</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="35">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="34">
         <v>8</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6176,27 +6203,27 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -6228,7 +6255,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -6257,7 +6284,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -6286,7 +6313,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -6315,7 +6342,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -6344,7 +6371,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -6371,7 +6398,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -6400,7 +6427,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -6417,19 +6444,19 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -6446,7 +6473,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>1</v>
       </c>
@@ -6461,7 +6488,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>2</v>
       </c>
@@ -6476,7 +6503,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>3</v>
       </c>
@@ -6493,7 +6520,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>4</v>
       </c>
@@ -6513,7 +6540,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>5</v>
       </c>
@@ -6533,7 +6560,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>6</v>
       </c>
@@ -6553,7 +6580,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>7</v>
       </c>
@@ -6573,12 +6600,12 @@
         <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G20" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>331</v>
       </c>
@@ -6589,7 +6616,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -6636,7 +6663,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>1</v>
       </c>
@@ -6679,7 +6706,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>2</v>
       </c>
@@ -6718,7 +6745,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -6755,7 +6782,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>4</v>
       </c>
@@ -6796,7 +6823,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>5</v>
       </c>
@@ -6827,7 +6854,7 @@
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>6</v>
       </c>
@@ -6856,7 +6883,7 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <v>7</v>
       </c>
@@ -6873,7 +6900,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="27"/>
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>
@@ -6902,20 +6929,20 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="5.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.41796875" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -6950,7 +6977,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6973,7 +7000,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6996,7 +7023,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7019,7 +7046,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7033,7 +7060,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7047,32 +7074,32 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -7095,7 +7122,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -7109,7 +7136,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -7123,7 +7150,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -7156,17 +7183,17 @@
       <selection activeCell="A2" sqref="A2:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -7189,7 +7216,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>6</v>
       </c>
@@ -7204,7 +7231,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>7</v>
       </c>
@@ -7219,7 +7246,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="10" t="s">
         <v>267</v>
@@ -7234,7 +7261,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>10</v>
       </c>
@@ -7251,7 +7278,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>15</v>
       </c>
@@ -7268,7 +7295,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>16</v>
       </c>
@@ -7285,7 +7312,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>17</v>
       </c>
@@ -7302,7 +7329,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>18</v>
       </c>
@@ -7335,54 +7362,54 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.68359375" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.578125" customWidth="1"/>
-    <col min="9" max="9" width="13.578125" customWidth="1"/>
-    <col min="10" max="10" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.68359375" customWidth="1"/>
-    <col min="17" max="17" width="6.41796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
+    <col min="17" max="17" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="10.68359375" customWidth="1"/>
-    <col min="22" max="22" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
+    <col min="22" max="22" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-    </row>
-    <row r="2" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+    </row>
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -7429,7 +7456,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>17</v>
       </c>
@@ -7468,7 +7495,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>18</v>
       </c>
@@ -7507,7 +7534,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>19</v>
       </c>
@@ -7540,7 +7567,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>22</v>
       </c>
@@ -7581,7 +7608,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>24</v>
       </c>
@@ -7622,7 +7649,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>26</v>
       </c>
@@ -7665,7 +7692,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>285</v>
       </c>
@@ -7708,7 +7735,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>286</v>
       </c>
@@ -7739,7 +7766,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>287</v>
       </c>
@@ -7773,7 +7800,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>288</v>
       </c>
@@ -7807,7 +7834,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>305</v>
       </c>
@@ -7833,7 +7860,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>302</v>
       </c>
@@ -7861,7 +7888,7 @@
       </c>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>300</v>
       </c>
@@ -7891,7 +7918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>301</v>
       </c>
@@ -7920,22 +7947,22 @@
       <c r="J16" s="16">
         <v>4</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="K16" s="39" t="s">
         <v>377</v>
       </c>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="Q16" s="32" t="s">
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="Q16" s="39" t="s">
         <v>378</v>
       </c>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
@@ -7989,7 +8016,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>303</v>
       </c>
@@ -8049,7 +8076,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>109</v>
       </c>
@@ -8107,7 +8134,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>110</v>
       </c>
@@ -8152,7 +8179,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>284</v>
       </c>
@@ -8191,7 +8218,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="22" t="s">
         <v>349</v>
@@ -8211,7 +8238,7 @@
       </c>
       <c r="J22" s="16"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="15" t="s">
         <v>351</v>
@@ -8230,23 +8257,23 @@
       <c r="J23" s="16">
         <v>7</v>
       </c>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" s="39"/>
-      <c r="K24" s="32" t="s">
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D24" s="38"/>
+      <c r="K24" s="39" t="s">
         <v>282</v>
       </c>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K25" t="s">
         <v>28</v>
       </c>
@@ -8263,7 +8290,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K26">
         <v>1</v>
       </c>
@@ -8280,7 +8307,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K27">
         <v>2</v>
       </c>
@@ -8297,7 +8324,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K28">
         <v>3</v>
       </c>
@@ -8314,7 +8341,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K29">
         <v>4</v>
       </c>
@@ -8331,7 +8358,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K30">
         <v>5</v>
       </c>
@@ -8348,7 +8375,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K31">
         <v>6</v>
       </c>
@@ -8365,16 +8392,16 @@
         <v>374</v>
       </c>
     </row>
-    <row r="34" spans="11:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="K34" s="32" t="s">
+    <row r="34" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K34" s="39" t="s">
         <v>371</v>
       </c>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-    </row>
-    <row r="35" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
+    </row>
+    <row r="35" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K35" t="s">
         <v>28</v>
       </c>
@@ -8391,7 +8418,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K36">
         <v>1</v>
       </c>
@@ -8408,7 +8435,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="37" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K37">
         <v>2</v>
       </c>
@@ -8425,16 +8452,16 @@
         <v>382</v>
       </c>
     </row>
-    <row r="40" spans="11:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="K40" s="32" t="s">
+    <row r="40" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K40" s="39" t="s">
         <v>372</v>
       </c>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-    </row>
-    <row r="41" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="39"/>
+    </row>
+    <row r="41" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K41" t="s">
         <v>28</v>
       </c>
@@ -8451,7 +8478,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K42">
         <v>1</v>
       </c>
@@ -8468,7 +8495,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K43">
         <v>2</v>
       </c>
@@ -8485,7 +8512,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="44" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K44">
         <v>3</v>
       </c>
@@ -8502,7 +8529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="11:15" x14ac:dyDescent="0.3">
       <c r="K45">
         <v>4</v>
       </c>
@@ -8557,18 +8584,18 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -8582,7 +8609,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -8596,7 +8623,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -8610,7 +8637,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
adds ECE night starting code
</commit_message>
<xml_diff>
--- a/harness/excelSheets/q20_dynoHarness.xlsx
+++ b/harness/excelSheets/q20_dynoHarness.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Desktop\formula\Q20\harness\excelSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\OneDrive\Documents\formula-BrentChampion\Q20\q20_git\harness\excelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3000B05-C1BC-4BE5-8A92-52C46E06558B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E3000B05-C1BC-4BE5-8A92-52C46E06558B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{508A155A-C352-420B-93E5-2C82B4088247}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="360" windowWidth="23232" windowHeight="12696" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDM" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="451">
   <si>
     <t>A11</t>
   </si>
@@ -1429,6 +1429,9 @@
   </si>
   <si>
     <t>To MD1</t>
+  </si>
+  <si>
+    <t>RapidHarness</t>
   </si>
 </sst>
 </file>
@@ -1680,7 +1683,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="97">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3966,19 +3982,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G23" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
-  <autoFilter ref="A1:G23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H23" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+  <autoFilter ref="A1:H23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
     <sortCondition ref="A1:A23"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Pin" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Signal" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Function" dataDxfId="91"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="To/From" dataDxfId="90"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Pin" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Signal" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Function" dataDxfId="92"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="To/From" dataDxfId="91"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="NOTES"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fuse" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{6DFCA7D8-4250-4344-80E1-1602B4F3D81B}" name="Voltage" dataDxfId="88"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fuse" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{6DFCA7D8-4250-4344-80E1-1602B4F3D81B}" name="Voltage" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{3138F25E-EC4D-4D70-A59A-5D3CF151BA58}" name="RapidHarness" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4030,38 +4047,38 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table11" displayName="Table11" ref="A1:G9" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table11" displayName="Table11" ref="A1:G9" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:G9" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Pin" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Signal" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Function" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="To/From" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Location" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="RH" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Pin" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Signal" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Function" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="To/From" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Location" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="RH" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="Notes" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table9" displayName="Table9" ref="A2:J23" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table9" displayName="Table9" ref="A2:J23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A2:J23" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Pin" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Signal" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Function" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="To/From" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Location" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="RH" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="Wired In" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="Connector A Female" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="Connector B" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Pin" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Signal" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Function" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="To/From" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Location" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="RH" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="Wired In" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="Connector A Female" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="Connector B" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4141,7 +4158,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table10" displayName="Table10" ref="A1:F16" totalsRowShown="0" headerRowDxfId="87" headerRowBorderDxfId="86" tableBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table10" displayName="Table10" ref="A1:F16" totalsRowShown="0" headerRowDxfId="88" headerRowBorderDxfId="87" tableBorderDxfId="86">
   <autoFilter ref="A1:F16" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F16">
     <sortCondition ref="A1:A16"/>
@@ -4151,7 +4168,7 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Signal"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Function"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Car Use"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="To/From" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="To/From" dataDxfId="85"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4187,17 +4204,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:E31" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:E31" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <autoFilter ref="A1:E31" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
     <sortCondition ref="B1:B31"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pin" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Signal" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Function" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="To/From" dataDxfId="78"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Notes" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pin" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Signal" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Function" dataDxfId="80"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="To/From" dataDxfId="79"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Notes" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4218,70 +4235,70 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table21" displayName="Table21" ref="A12:E19" totalsRowShown="0" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75" tableBorderDxfId="73" totalsRowBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table21" displayName="Table21" ref="A12:E19" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="A12:E19" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Pin" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Signal" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Function" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="To/From" dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Location" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Pin" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Signal" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Function" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="To/From" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Location" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table13" displayName="Table13" ref="A2:E9" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table13" displayName="Table13" ref="A2:E9" totalsRowShown="0" headerRowDxfId="67" dataDxfId="65" headerRowBorderDxfId="66" tableBorderDxfId="64" totalsRowBorderDxfId="63">
   <autoFilter ref="A2:E9" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Pin" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Signal" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Function" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="To/From" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Location" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Pin" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Signal" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Function" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="To/From" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Location" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table1320" displayName="Table1320" ref="A26:E34" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table1320" displayName="Table1320" ref="A26:E34" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="A26:E34" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Pin" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Signal" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Function" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="To/From" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Location" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Pin" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Signal" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Function" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="To/From" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Location" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table132025" displayName="Table132025" ref="G26:K32" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table132025" displayName="Table132025" ref="G26:K32" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="G26:K32" xr:uid="{00000000-0009-0000-0100-000018000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Pin" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Signal" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Function" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="To/From" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Location" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Pin" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Signal" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Function" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="To/From" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Location" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table13202527" displayName="Table13202527" ref="M26:Q32" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table13202527" displayName="Table13202527" ref="M26:Q32" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="M26:Q32" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Pin" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Signal" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Function" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="To/From" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Location" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Pin" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Signal" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Function" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="To/From" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Location" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4568,30 +4585,30 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.68359375" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="14.05078125" style="30" customWidth="1"/>
-    <col min="8" max="8" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="30" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>28</v>
       </c>
@@ -4612,12 +4629,15 @@
       </c>
       <c r="G1" s="37" t="s">
         <v>386</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>450</v>
       </c>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -4637,11 +4657,14 @@
         <v>13</v>
       </c>
       <c r="G2" s="31"/>
+      <c r="H2" s="31" t="s">
+        <v>125</v>
+      </c>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -4661,11 +4684,14 @@
         <v>14</v>
       </c>
       <c r="G3" s="31"/>
+      <c r="H3" s="31" t="s">
+        <v>125</v>
+      </c>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -4685,11 +4711,14 @@
         <v>14</v>
       </c>
       <c r="G4" s="31"/>
+      <c r="H4" s="31" t="s">
+        <v>125</v>
+      </c>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -4706,11 +4735,12 @@
         <v>13</v>
       </c>
       <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -4730,11 +4760,12 @@
         <v>14</v>
       </c>
       <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -4751,11 +4782,12 @@
         <v>13</v>
       </c>
       <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4775,11 +4807,12 @@
         <v>14</v>
       </c>
       <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -4796,11 +4829,12 @@
         <v>14</v>
       </c>
       <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -4817,11 +4851,12 @@
         <v>14</v>
       </c>
       <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -4836,11 +4871,12 @@
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -4855,11 +4891,12 @@
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -4876,11 +4913,12 @@
         <v>159</v>
       </c>
       <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -4895,11 +4933,12 @@
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -4911,11 +4950,12 @@
       </c>
       <c r="F15" s="30"/>
       <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -4930,11 +4970,12 @@
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -4951,11 +4992,12 @@
         <v>13</v>
       </c>
       <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -4975,11 +5017,12 @@
         <v>13</v>
       </c>
       <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -4996,11 +5039,12 @@
         <v>159</v>
       </c>
       <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -5013,11 +5057,12 @@
       <c r="D20" s="16"/>
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -5032,11 +5077,12 @@
       </c>
       <c r="F21" s="30"/>
       <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -5051,11 +5097,12 @@
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>228</v>
       </c>
@@ -5073,201 +5120,202 @@
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I39"/>
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I40"/>
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I41"/>
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I42"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I45"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I46"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I47"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I48"/>
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I49"/>
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I50"/>
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I51"/>
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I56"/>
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I57"/>
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I58"/>
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I59"/>
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I60"/>
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I61"/>
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="9:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I62"/>
       <c r="J62"/>
       <c r="K62"/>
@@ -5289,14 +5337,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.3125" customWidth="1"/>
-    <col min="2" max="2" width="17.26171875" customWidth="1"/>
-    <col min="3" max="3" width="26.7890625" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -5313,7 +5361,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>428</v>
       </c>
@@ -5324,7 +5372,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>429</v>
       </c>
@@ -5332,7 +5380,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>430</v>
       </c>
@@ -5340,7 +5388,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>431</v>
       </c>
@@ -5348,12 +5396,12 @@
         <v>439</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>433</v>
       </c>
@@ -5368,7 +5416,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" t="s">
@@ -5378,15 +5426,15 @@
         <v>445</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>289</v>
       </c>
@@ -5398,32 +5446,32 @@
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>434</v>
       </c>
       <c r="B15" s="18"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -5446,23 +5494,23 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="29.62890625" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.41796875" customWidth="1"/>
-    <col min="9" max="10" width="10.83984375" customWidth="1"/>
-    <col min="11" max="11" width="22.26171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -5483,7 +5531,7 @@
       </c>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7</v>
       </c>
@@ -5500,7 +5548,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -5517,7 +5565,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -5534,7 +5582,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17</v>
       </c>
@@ -5554,7 +5602,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>18</v>
       </c>
@@ -5574,7 +5622,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>23</v>
       </c>
@@ -5591,7 +5639,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>24</v>
       </c>
@@ -5608,7 +5656,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
@@ -5622,7 +5670,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>28</v>
       </c>
@@ -5636,7 +5684,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>67</v>
       </c>
@@ -5652,7 +5700,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>68</v>
       </c>
@@ -5665,7 +5713,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>73</v>
       </c>
@@ -5682,7 +5730,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>74</v>
       </c>
@@ -5699,7 +5747,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>77</v>
       </c>
@@ -5714,7 +5762,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>78</v>
       </c>
@@ -5727,7 +5775,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>127</v>
       </c>
@@ -5735,7 +5783,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>415</v>
       </c>
@@ -5743,7 +5791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>246</v>
       </c>
@@ -5765,19 +5813,19 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7890625" customWidth="1"/>
-    <col min="2" max="2" width="23.41796875" customWidth="1"/>
-    <col min="3" max="3" width="23.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.89453125" customWidth="1"/>
-    <col min="5" max="5" width="26.26171875" customWidth="1"/>
-    <col min="6" max="6" width="24.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>28</v>
       </c>
@@ -5795,7 +5843,7 @@
       </c>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>43</v>
       </c>
@@ -5810,7 +5858,7 @@
       </c>
       <c r="E2" s="26"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>37</v>
       </c>
@@ -5825,7 +5873,7 @@
       </c>
       <c r="E3" s="26"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>33</v>
       </c>
@@ -5840,7 +5888,7 @@
       </c>
       <c r="E4" s="26"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>38</v>
       </c>
@@ -5853,7 +5901,7 @@
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>99</v>
       </c>
@@ -5866,7 +5914,7 @@
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>100</v>
       </c>
@@ -5879,7 +5927,7 @@
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>46</v>
       </c>
@@ -5893,7 +5941,7 @@
       <c r="E8" s="26"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>47</v>
       </c>
@@ -5906,7 +5954,7 @@
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>94</v>
       </c>
@@ -5921,7 +5969,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>36</v>
       </c>
@@ -5934,7 +5982,7 @@
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>32</v>
       </c>
@@ -5947,7 +5995,7 @@
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>42</v>
       </c>
@@ -5960,7 +6008,7 @@
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>102</v>
       </c>
@@ -5973,7 +6021,7 @@
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>101</v>
       </c>
@@ -5986,7 +6034,7 @@
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>91</v>
       </c>
@@ -5999,7 +6047,7 @@
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>39</v>
       </c>
@@ -6012,7 +6060,7 @@
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>41</v>
       </c>
@@ -6025,7 +6073,7 @@
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>98</v>
       </c>
@@ -6041,7 +6089,7 @@
       <c r="E19" s="26"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>30</v>
       </c>
@@ -6055,7 +6103,7 @@
       <c r="E20" s="26"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>93</v>
       </c>
@@ -6070,7 +6118,7 @@
       </c>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>44</v>
       </c>
@@ -6085,7 +6133,7 @@
       </c>
       <c r="E22" s="26"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>45</v>
       </c>
@@ -6100,7 +6148,7 @@
       </c>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>96</v>
       </c>
@@ -6115,7 +6163,7 @@
       </c>
       <c r="E24" s="26"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>97</v>
       </c>
@@ -6130,7 +6178,7 @@
       </c>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>95</v>
       </c>
@@ -6143,7 +6191,7 @@
       <c r="D26" s="26"/>
       <c r="E26" s="26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>34</v>
       </c>
@@ -6156,7 +6204,7 @@
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>35</v>
       </c>
@@ -6169,7 +6217,7 @@
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>92</v>
       </c>
@@ -6182,7 +6230,7 @@
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>31</v>
       </c>
@@ -6197,7 +6245,7 @@
       </c>
       <c r="E30" s="26"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>40</v>
       </c>
@@ -6229,19 +6277,19 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26171875" customWidth="1"/>
-    <col min="2" max="2" width="17.9453125" customWidth="1"/>
-    <col min="3" max="3" width="14.1015625" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>28</v>
       </c>
@@ -6261,7 +6309,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <v>1</v>
       </c>
@@ -6271,7 +6319,7 @@
       <c r="E3" s="35"/>
       <c r="F3" s="35"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>2</v>
       </c>
@@ -6281,7 +6329,7 @@
       <c r="E4" s="35"/>
       <c r="F4" s="35"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
         <v>3</v>
       </c>
@@ -6291,7 +6339,7 @@
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <v>4</v>
       </c>
@@ -6301,7 +6349,7 @@
       <c r="E6" s="35"/>
       <c r="F6" s="35"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <v>5</v>
       </c>
@@ -6311,7 +6359,7 @@
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <v>6</v>
       </c>
@@ -6321,7 +6369,7 @@
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="34">
         <v>7</v>
       </c>
@@ -6331,7 +6379,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>8</v>
       </c>
@@ -6341,12 +6389,12 @@
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>28</v>
       </c>
@@ -6366,7 +6414,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>1</v>
       </c>
@@ -6376,7 +6424,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <v>2</v>
       </c>
@@ -6386,7 +6434,7 @@
       <c r="E15" s="35"/>
       <c r="F15" s="35"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>3</v>
       </c>
@@ -6396,7 +6444,7 @@
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="34">
         <v>4</v>
       </c>
@@ -6406,7 +6454,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="35"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>5</v>
       </c>
@@ -6416,7 +6464,7 @@
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <v>6</v>
       </c>
@@ -6426,7 +6474,7 @@
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>7</v>
       </c>
@@ -6436,7 +6484,7 @@
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="34">
         <v>8</v>
       </c>
@@ -6460,27 +6508,27 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -6512,7 +6560,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -6541,7 +6589,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -6570,7 +6618,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -6599,7 +6647,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -6628,7 +6676,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -6655,7 +6703,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -6684,7 +6732,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -6701,19 +6749,19 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -6730,7 +6778,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>1</v>
       </c>
@@ -6745,7 +6793,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>2</v>
       </c>
@@ -6760,7 +6808,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>3</v>
       </c>
@@ -6777,7 +6825,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>4</v>
       </c>
@@ -6797,7 +6845,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>5</v>
       </c>
@@ -6817,7 +6865,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>6</v>
       </c>
@@ -6837,7 +6885,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>7</v>
       </c>
@@ -6857,12 +6905,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>328</v>
       </c>
@@ -6873,7 +6921,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -6920,7 +6968,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>1</v>
       </c>
@@ -6963,7 +7011,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>2</v>
       </c>
@@ -7002,7 +7050,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>3</v>
       </c>
@@ -7039,7 +7087,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>4</v>
       </c>
@@ -7080,7 +7128,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>5</v>
       </c>
@@ -7111,7 +7159,7 @@
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>6</v>
       </c>
@@ -7140,7 +7188,7 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
         <v>7</v>
       </c>
@@ -7157,7 +7205,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="27"/>
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>
@@ -7186,20 +7234,20 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="5.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.41796875" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -7234,7 +7282,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7257,7 +7305,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7280,7 +7328,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7303,7 +7351,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7317,7 +7365,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7331,32 +7379,32 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -7379,7 +7427,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -7393,7 +7441,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -7407,7 +7455,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -7440,17 +7488,17 @@
       <selection activeCell="A2" sqref="A2:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -7473,7 +7521,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>6</v>
       </c>
@@ -7488,7 +7536,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>7</v>
       </c>
@@ -7503,7 +7551,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="10" t="s">
         <v>265</v>
@@ -7518,7 +7566,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>10</v>
       </c>
@@ -7535,7 +7583,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>15</v>
       </c>
@@ -7552,7 +7600,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>16</v>
       </c>
@@ -7569,7 +7617,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>17</v>
       </c>
@@ -7586,7 +7634,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>18</v>
       </c>
@@ -7619,30 +7667,30 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.68359375" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.578125" customWidth="1"/>
-    <col min="9" max="9" width="13.578125" customWidth="1"/>
-    <col min="10" max="10" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.68359375" customWidth="1"/>
-    <col min="17" max="17" width="6.41796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="10.68359375" customWidth="1"/>
-    <col min="22" max="22" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>199</v>
       </c>
@@ -7666,7 +7714,7 @@
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
     </row>
-    <row r="2" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -7713,7 +7761,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>17</v>
       </c>
@@ -7752,7 +7800,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>18</v>
       </c>
@@ -7791,7 +7839,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>19</v>
       </c>
@@ -7824,7 +7872,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>22</v>
       </c>
@@ -7865,7 +7913,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>24</v>
       </c>
@@ -7906,7 +7954,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>26</v>
       </c>
@@ -7949,7 +7997,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>283</v>
       </c>
@@ -7992,7 +8040,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>284</v>
       </c>
@@ -8023,7 +8071,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>285</v>
       </c>
@@ -8057,7 +8105,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>286</v>
       </c>
@@ -8091,7 +8139,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>303</v>
       </c>
@@ -8117,7 +8165,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>300</v>
       </c>
@@ -8145,7 +8193,7 @@
       </c>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>298</v>
       </c>
@@ -8175,7 +8223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>299</v>
       </c>
@@ -8219,7 +8267,7 @@
       <c r="T16" s="39"/>
       <c r="U16" s="39"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
@@ -8273,7 +8321,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>301</v>
       </c>
@@ -8333,7 +8381,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>107</v>
       </c>
@@ -8391,7 +8439,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>108</v>
       </c>
@@ -8436,7 +8484,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>282</v>
       </c>
@@ -8475,7 +8523,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="22" t="s">
         <v>346</v>
@@ -8495,7 +8543,7 @@
       </c>
       <c r="J22" s="16"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="15" t="s">
         <v>348</v>
@@ -8520,7 +8568,7 @@
       <c r="N23" s="39"/>
       <c r="O23" s="39"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D24" s="38"/>
       <c r="K24" s="39" t="s">
         <v>280</v>
@@ -8530,7 +8578,7 @@
       <c r="N24" s="39"/>
       <c r="O24" s="39"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
         <v>28</v>
       </c>
@@ -8547,7 +8595,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K26">
         <v>1</v>
       </c>
@@ -8564,7 +8612,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K27">
         <v>2</v>
       </c>
@@ -8581,7 +8629,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K28">
         <v>3</v>
       </c>
@@ -8598,7 +8646,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K29">
         <v>4</v>
       </c>
@@ -8615,7 +8663,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K30">
         <v>5</v>
       </c>
@@ -8632,7 +8680,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K31">
         <v>6</v>
       </c>
@@ -8649,7 +8697,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="34" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K34" s="39" t="s">
         <v>368</v>
       </c>
@@ -8658,7 +8706,7 @@
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
     </row>
-    <row r="35" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K35" t="s">
         <v>28</v>
       </c>
@@ -8675,7 +8723,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K36">
         <v>1</v>
       </c>
@@ -8692,7 +8740,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="37" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K37">
         <v>2</v>
       </c>
@@ -8709,7 +8757,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="40" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K40" s="39" t="s">
         <v>369</v>
       </c>
@@ -8718,7 +8766,7 @@
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
     </row>
-    <row r="41" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K41" t="s">
         <v>28</v>
       </c>
@@ -8735,7 +8783,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K42">
         <v>1</v>
       </c>
@@ -8752,7 +8800,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K43">
         <v>2</v>
       </c>
@@ -8769,7 +8817,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="44" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K44">
         <v>3</v>
       </c>
@@ -8786,7 +8834,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="11:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K45">
         <v>4</v>
       </c>
@@ -8841,18 +8889,18 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -8866,7 +8914,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -8880,7 +8928,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -8894,7 +8942,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>142</v>
       </c>

</xml_diff>